<commit_message>
Complete login process with custom env and browser
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/Login.xlsx
+++ b/src/main/resources/modules/Login.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="4380" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="20370" yWindow="4830" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="19" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="58">
   <si>
     <t>Action</t>
   </si>
@@ -193,12 +193,18 @@
   <si>
     <t>Verify Login in production</t>
   </si>
+  <si>
+    <t>TestEnvName</t>
+  </si>
+  <si>
+    <t>sample101,sample102,sample103,sample104</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -249,8 +255,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,6 +304,12 @@
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FF4472C4"/>
       </patternFill>
     </fill>
   </fills>
@@ -429,7 +450,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -553,6 +574,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -562,9 +586,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -982,22 +1008,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
     <col min="3" max="3" width="82.7109375" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" width="49.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
@@ -1022,8 +1049,11 @@
       <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="I1" s="25" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="24" customFormat="1">
       <c r="A2" s="21"/>
       <c r="B2" s="22"/>
       <c r="C2" s="21" t="s">
@@ -1031,8 +1061,9 @@
       </c>
       <c r="D2" s="21"/>
       <c r="E2" s="23"/>
+      <c r="I2" s="49"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1051,6 +1082,33 @@
       <c r="F3" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="I3" s="50" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="I4" s="51"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="I5" s="51"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="I6" s="51"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="I7" s="51"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="I8" s="51"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="I9" s="50"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="I10" s="51"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="I11" s="51"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1062,11 +1120,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="1" customWidth="1"/>
@@ -1081,7 +1139,7 @@
     <col min="11" max="11" width="85.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16384" s="1" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
@@ -1119,21 +1177,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:16384" s="29" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16384" s="29" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="31"/>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="48"/>
       <c r="F2" s="33"/>
       <c r="G2" s="32"/>
       <c r="H2" s="31"/>
       <c r="I2" s="30"/>
       <c r="J2" s="30"/>
     </row>
-    <row r="3" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16384">
       <c r="A3" s="8" t="s">
         <v>26</v>
       </c>
@@ -1163,7 +1221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16384">
       <c r="A4" s="8" t="s">
         <v>26</v>
       </c>
@@ -1196,7 +1254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16384">
       <c r="A5" s="8" t="s">
         <v>26</v>
       </c>
@@ -1231,7 +1289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16384">
       <c r="A6" s="8" t="s">
         <v>26</v>
       </c>
@@ -1266,7 +1324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16384">
       <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
@@ -1301,7 +1359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16384">
       <c r="A8" s="8" t="s">
         <v>26</v>
       </c>
@@ -1330,14 +1388,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16384">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="14">
         <v>7</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="45" t="s">
         <v>54</v>
       </c>
       <c r="D9" s="14" t="s">
@@ -17738,7 +17796,7 @@
       <c r="XFC9" s="14"/>
       <c r="XFD9" s="14"/>
     </row>
-    <row r="10" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16384">
       <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
@@ -17774,7 +17832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16384" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16384">
       <c r="A11" s="8"/>
       <c r="B11" s="39"/>
       <c r="D11" s="40"/>

</xml_diff>

<commit_message>
Update Email process for passed TcReport only
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/Login.xlsx
+++ b/src/main/resources/modules/Login.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="6180" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="20370" yWindow="6630" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="19" r:id="rId1"/>
@@ -197,7 +197,7 @@
     <t>TestEnvName</t>
   </si>
   <si>
-    <t>sample101</t>
+    <t>TCEnv101</t>
   </si>
 </sst>
 </file>
@@ -1011,7 +1011,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>